<commit_message>
modified git ignore file
</commit_message>
<xml_diff>
--- a/Personal accounting office.xlsx
+++ b/Personal accounting office.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal accounting office\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal accounting office\Github_Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5850" windowWidth="25200" windowHeight="12015" tabRatio="907" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="25200" windowHeight="12015" tabRatio="907" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="چک نویس" sheetId="22" r:id="rId1"/>
@@ -1729,6 +1729,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1736,9 +1739,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -1754,14 +1754,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
       <font>
@@ -1770,13 +1767,32 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
       <font>
@@ -1785,13 +1801,38 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
       <font>
@@ -1911,25 +1952,15 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="165" formatCode="#,##0_-[$ريال-429]"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
@@ -1959,6 +1990,19 @@
     <dxf>
       <font>
         <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1972,107 +2016,12 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="#,##0_-[$ريال-429]"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
@@ -2091,13 +2040,18 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
@@ -2306,6 +2260,52 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
@@ -4129,44 +4129,44 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Accounts_and_ReceiversAndPayers_AppendTabel" displayName="Accounts_and_ReceiversAndPayers_AppendTabel" ref="C3:E19" tableType="queryTable" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="C3:E19"/>
   <tableColumns count="3">
-    <tableColumn id="4" uniqueName="4" name="Accounts" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="5" uniqueName="5" name="ReceiversAndPayers" queryTableFieldId="2" dataDxfId="1"/>
-    <tableColumn id="6" uniqueName="6" name="Accounts and ReceiversAndPayers" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" uniqueName="4" name="Accounts" queryTableFieldId="1" dataDxfId="33"/>
+    <tableColumn id="5" uniqueName="5" name="ReceiversAndPayers" queryTableFieldId="2" dataDxfId="32"/>
+    <tableColumn id="6" uniqueName="6" name="Accounts and ReceiversAndPayers" queryTableFieldId="3" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table38.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="PersonsTable" displayName="PersonsTable" ref="A5:I6" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="PersonsTable" displayName="PersonsTable" ref="A5:I6" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A5:I6"/>
   <tableColumns count="9">
-    <tableColumn id="6" name="ID" dataDxfId="31"/>
-    <tableColumn id="1" name="افراد" dataDxfId="30"/>
-    <tableColumn id="2" name="کد ملی" dataDxfId="29"/>
-    <tableColumn id="3" name="شماره تماس" dataDxfId="28"/>
-    <tableColumn id="4" name="آدرس ایمیل" dataDxfId="27" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="سایت اینترنتی" dataDxfId="26"/>
-    <tableColumn id="7" name="آدرس محل کار" dataDxfId="25"/>
-    <tableColumn id="8" name="آدرس منزل" dataDxfId="24"/>
-    <tableColumn id="9" name="توضیحات" dataDxfId="23"/>
+    <tableColumn id="6" name="ID" dataDxfId="28"/>
+    <tableColumn id="1" name="افراد" dataDxfId="27"/>
+    <tableColumn id="2" name="کد ملی" dataDxfId="26"/>
+    <tableColumn id="3" name="شماره تماس" dataDxfId="25"/>
+    <tableColumn id="4" name="آدرس ایمیل" dataDxfId="24" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="سایت اینترنتی" dataDxfId="23"/>
+    <tableColumn id="7" name="آدرس محل کار" dataDxfId="22"/>
+    <tableColumn id="8" name="آدرس منزل" dataDxfId="21"/>
+    <tableColumn id="9" name="توضیحات" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FinancialAccountsTable" displayName="FinancialAccountsTable" ref="A12:H18" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FinancialAccountsTable" displayName="FinancialAccountsTable" ref="A12:H18" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A12:H17"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="ID" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="10"/>
-    <tableColumn id="2" name="نام حساب" dataDxfId="19" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="نوع حساب" dataDxfId="18" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="موجودی اولیه" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="7"/>
-    <tableColumn id="5" name="شماره حساب" totalsRowDxfId="6"/>
-    <tableColumn id="6" name="شماره کارت" totalsRowDxfId="5"/>
-    <tableColumn id="7" name="تاریخ انقضاء کارت" totalsRowDxfId="4"/>
-    <tableColumn id="8" name="CVV2" totalsRowDxfId="3"/>
+    <tableColumn id="1" name="ID" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="2" name="نام حساب" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="3" name="نوع حساب" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="4" name="موجودی اولیه" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="5" name="شماره حساب" totalsRowDxfId="9"/>
+    <tableColumn id="6" name="شماره کارت" totalsRowDxfId="8"/>
+    <tableColumn id="7" name="تاریخ انقضاء کارت" totalsRowDxfId="7"/>
+    <tableColumn id="8" name="CVV2" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4183,20 +4183,20 @@
 </file>
 
 <file path=xl/tables/table40.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TypeOfExpenditureTable" displayName="TypeOfExpenditureTable" ref="A3:A6" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TypeOfExpenditureTable" displayName="TypeOfExpenditureTable" ref="A3:A6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A3:A6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="نوع خرج" dataDxfId="14"/>
+    <tableColumn id="1" name="نوع خرج" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table41.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TypeOfTransactionTable" displayName="TypeOfTransactionTable" ref="B3:B6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TypeOfTransactionTable" displayName="TypeOfTransactionTable" ref="B3:B6" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="B3:B6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="نوع تراکنش" dataDxfId="11"/>
+    <tableColumn id="1" name="نوع تراکنش" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4920,10 +4920,10 @@
     </row>
     <row r="2" spans="1:23" s="45" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="103" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="102"/>
+      <c r="B3" s="103"/>
       <c r="D3" s="45"/>
       <c r="F3" s="45"/>
       <c r="H3" s="45"/>
@@ -5348,10 +5348,10 @@
       <c r="AC3" s="92"/>
     </row>
     <row r="4" spans="1:55" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="104" t="s">
         <v>177</v>
       </c>
-      <c r="B4" s="103"/>
+      <c r="B4" s="104"/>
       <c r="D4" s="47" t="s">
         <v>195</v>
       </c>
@@ -7483,7 +7483,7 @@
       <c r="B6" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="104">
+      <c r="C6" s="101">
         <v>1111111111</v>
       </c>
       <c r="D6" s="49" t="s">
@@ -7966,7 +7966,7 @@
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8061,10 +8061,10 @@
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="88"/>
-      <c r="I3" s="101" t="s">
+      <c r="I3" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="J3" s="101"/>
+      <c r="J3" s="102"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="32"/>

</xml_diff>

<commit_message>
Remaining calculation test in Excel file
</commit_message>
<xml_diff>
--- a/Personal accounting office.xlsx
+++ b/Personal accounting office.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7200" windowWidth="25200" windowHeight="12015" tabRatio="907" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="7650" windowWidth="25200" windowHeight="12015" tabRatio="907" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="چک نویس" sheetId="22" r:id="rId1"/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="352">
   <si>
     <t>تاریخ</t>
   </si>
@@ -1152,6 +1152,12 @@
   </si>
   <si>
     <t>مجموع کل انتقال‌ها:</t>
+  </si>
+  <si>
+    <t>cell</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -1259,11 +1265,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1276,6 +1284,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1841,15 +1850,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1868,6 +1868,15 @@
     <xf numFmtId="165" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1875,6 +1884,152 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="165">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1897,6 +2052,25 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="#,##0_-[$ريال-429]"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
@@ -1939,31 +2113,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="#,##0_-[$ريال-429]"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
@@ -1983,9 +2133,9 @@
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="1"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
@@ -2108,25 +2258,15 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="165" formatCode="#,##0_-[$ريال-429]"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
@@ -2156,18 +2296,13 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
@@ -2184,43 +2319,15 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="#,##0_-[$ريال-429]"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="#,##0_-[$ريال-429]"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="#,##0_-[$ريال-429]"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
@@ -2239,13 +2346,18 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
@@ -2297,93 +2409,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
       <font>
@@ -3815,21 +3840,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="165" formatCode="#,##0_-[$ريال-429]"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
       <protection locked="0" hidden="0"/>
@@ -4040,424 +4050,424 @@
     <tableColumn id="8" name="مبلغ (ریال)" dataDxfId="154"/>
     <tableColumn id="9" name="پرداخت کننده" dataDxfId="153"/>
     <tableColumn id="10" name="دریافت کننده" dataDxfId="152"/>
-    <tableColumn id="11" name="مانده حساب‌ها" dataDxfId="151"/>
-    <tableColumn id="12" name="نوع خرج" dataDxfId="150"/>
-    <tableColumn id="13" name="شرح" dataDxfId="149"/>
+    <tableColumn id="11" name="مانده حساب‌ها" dataDxfId="0"/>
+    <tableColumn id="12" name="نوع خرج" dataDxfId="151"/>
+    <tableColumn id="13" name="شرح" dataDxfId="150"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="RightsTable" displayName="RightsTable" ref="D5:D6" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="RightsTable" displayName="RightsTable" ref="D5:D6" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123">
   <autoFilter ref="D5:D6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="حقوق" dataDxfId="121"/>
+    <tableColumn id="1" name="حقوق" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="CostGroupsTable" displayName="CostGroupsTable" ref="A5:B29" totalsRowShown="0" headerRowDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="CostGroupsTable" displayName="CostGroupsTable" ref="A5:B29" totalsRowShown="0" headerRowDxfId="121">
   <autoFilter ref="A5:B29"/>
   <sortState ref="A5:B28">
     <sortCondition ref="B4:B28"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="کد گروه هزینه" dataDxfId="119"/>
-    <tableColumn id="2" name="نام گروه هزینه" dataDxfId="118"/>
+    <tableColumn id="1" name="کد گروه هزینه" dataDxfId="120"/>
+    <tableColumn id="2" name="نام گروه هزینه" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="TravelCostsTable" displayName="TravelCostsTable" ref="F4:F13" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="TravelCostsTable" displayName="TravelCostsTable" ref="F4:F13" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117">
   <autoFilter ref="F4:F13"/>
   <sortState ref="F4:F12">
     <sortCondition ref="F3:F12"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="ایاب و ذهاب" dataDxfId="115"/>
+    <tableColumn id="1" name="ایاب و ذهاب" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="NetworkCostsTable" displayName="NetworkCostsTable" ref="D4:D8" totalsRowShown="0" headerRowDxfId="114" dataDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="NetworkCostsTable" displayName="NetworkCostsTable" ref="D4:D8" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114">
   <autoFilter ref="D4:D8"/>
   <sortState ref="D4:D7">
     <sortCondition ref="D3:D7"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="ارتباطات" dataDxfId="112"/>
+    <tableColumn id="1" name="ارتباطات" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="HealthCareCostsTable" displayName="HealthCareCostsTable" ref="H4:H9" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="HealthCareCostsTable" displayName="HealthCareCostsTable" ref="H4:H9" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
   <autoFilter ref="H4:H9"/>
   <sortState ref="H4:H8">
     <sortCondition ref="H3:H8"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="بهداشت و درمان" dataDxfId="109"/>
+    <tableColumn id="1" name="بهداشت و درمان" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="PersonalCleaningCostsTable" displayName="PersonalCleaningCostsTable" ref="J4:J9" totalsRowShown="0" headerRowDxfId="108" dataDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="PersonalCleaningCostsTable" displayName="PersonalCleaningCostsTable" ref="J4:J9" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
   <autoFilter ref="J4:J9"/>
   <sortState ref="J4:J8">
     <sortCondition ref="J3:J8"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="بهداشت و نظافت فردی" dataDxfId="106"/>
+    <tableColumn id="1" name="بهداشت و نظافت فردی" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="EnvironmentalHealthCostsTable" displayName="EnvironmentalHealthCostsTable" ref="L4:L6" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="EnvironmentalHealthCostsTable" displayName="EnvironmentalHealthCostsTable" ref="L4:L6" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
   <autoFilter ref="L4:L6"/>
   <sortState ref="L4:L5">
     <sortCondition ref="L3:L5"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="بهداشت و نظافت محیط" dataDxfId="103"/>
+    <tableColumn id="1" name="بهداشت و نظافت محیط" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="InsuranceCostsTable" displayName="InsuranceCostsTable" ref="N4:N8" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="InsuranceCostsTable" displayName="InsuranceCostsTable" ref="N4:N8" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
   <autoFilter ref="N4:N8"/>
   <sortState ref="N4:N7">
     <sortCondition ref="N3:N7"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="بیمه" dataDxfId="100"/>
+    <tableColumn id="1" name="بیمه" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="InstallmentPaymentCostsTable" displayName="InstallmentPaymentCostsTable" ref="P4:P6" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="InstallmentPaymentCostsTable" displayName="InstallmentPaymentCostsTable" ref="P4:P6" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
   <autoFilter ref="P4:P6"/>
   <sortState ref="P4">
     <sortCondition ref="P3:P4"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="پرداخت اقساط" dataDxfId="97"/>
+    <tableColumn id="1" name="پرداخت اقساط" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="CostsOfClothingAndFootwearTable" displayName="CostsOfClothingAndFootwearTable" ref="R4:R8" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="CostsOfClothingAndFootwearTable" displayName="CostsOfClothingAndFootwearTable" ref="R4:R8" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="R4:R8"/>
   <sortState ref="R4:R7">
     <sortCondition ref="R3:R7"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="پوشاک و کفش" dataDxfId="94"/>
+    <tableColumn id="1" name="پوشاک و کفش" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="RevenueGroupTable" displayName="RevenueGroupTable" ref="A4:B12" totalsRowShown="0" headerRowDxfId="148" dataDxfId="147">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="RevenueGroupTable" displayName="RevenueGroupTable" ref="A4:B12" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
   <autoFilter ref="A4:B12"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="کد گروه درآمدی" dataDxfId="146"/>
-    <tableColumn id="2" name="نام گروه درآمد" dataDxfId="145"/>
+    <tableColumn id="1" name="کد گروه درآمدی" dataDxfId="147"/>
+    <tableColumn id="2" name="نام گروه درآمد" dataDxfId="146"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="CarCostsTable" displayName="CarCostsTable" ref="T4:T9" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="CarCostsTable" displayName="CarCostsTable" ref="T4:T9" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
   <autoFilter ref="T4:T9"/>
   <sortState ref="T4:T8">
     <sortCondition ref="T3:T8"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="خودرو" dataDxfId="91"/>
+    <tableColumn id="1" name="خودرو" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="CostsOfFoodAndBeveragesTable" displayName="CostsOfFoodAndBeveragesTable" ref="V4:V8" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="CostsOfFoodAndBeveragesTable" displayName="CostsOfFoodAndBeveragesTable" ref="V4:V8" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90">
   <autoFilter ref="V4:V8"/>
   <sortState ref="V4:V7">
     <sortCondition ref="V3:V7"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="خوراکی‌ها و آشامیدنی‌ها" dataDxfId="88"/>
+    <tableColumn id="1" name="خوراکی‌ها و آشامیدنی‌ها" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="CharityAndCulturalExpensesTable" displayName="CharityAndCulturalExpensesTable" ref="X4:X6" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="CharityAndCulturalExpensesTable" displayName="CharityAndCulturalExpensesTable" ref="X4:X6" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87">
   <autoFilter ref="X4:X6"/>
   <sortState ref="X4">
     <sortCondition ref="X3:X4"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="خیریه و امور فرهنگی" dataDxfId="85"/>
+    <tableColumn id="1" name="خیریه و امور فرهنگی" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="TobaccoCostsTable" displayName="TobaccoCostsTable" ref="Z4:Z6" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="TobaccoCostsTable" displayName="TobaccoCostsTable" ref="Z4:Z6" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
   <autoFilter ref="Z4:Z6"/>
   <sortState ref="Z4:Z5">
     <sortCondition ref="Z3:Z5"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="دخانیات" dataDxfId="82"/>
+    <tableColumn id="1" name="دخانیات" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="BicycleCostsTable" displayName="BicycleCostsTable" ref="AB4:AB6" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="BicycleCostsTable" displayName="BicycleCostsTable" ref="AB4:AB6" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
   <autoFilter ref="AB4:AB6"/>
   <sortState ref="AB4:AB5">
     <sortCondition ref="AB3:AB5"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="دوچرخه" dataDxfId="79"/>
+    <tableColumn id="1" name="دوچرخه" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="CostsOfCapitalJewelryTable" displayName="CostsOfCapitalJewelryTable" ref="AD4:AD8" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="CostsOfCapitalJewelryTable" displayName="CostsOfCapitalJewelryTable" ref="AD4:AD8" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
   <autoFilter ref="AD4:AD8"/>
   <sortState ref="AD4:AD7">
     <sortCondition ref="AD3:AD7"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="زیورآلات سرمایه" dataDxfId="76"/>
+    <tableColumn id="1" name="زیورآلات سرمایه" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Non_CapitalJewelryCostsTable" displayName="Non_CapitalJewelryCostsTable" ref="AF4:AF6" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Non_CapitalJewelryCostsTable" displayName="Non_CapitalJewelryCostsTable" ref="AF4:AF6" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <autoFilter ref="AF4:AF6"/>
   <sortState ref="AF4">
     <sortCondition ref="AF3:AF4"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name=" زیورآلات غیر سرمایه" dataDxfId="73"/>
+    <tableColumn id="1" name=" زیورآلات غیر سرمایه" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="InvestmentCostsTable" displayName="InvestmentCostsTable" ref="AH4:AH6" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="InvestmentCostsTable" displayName="InvestmentCostsTable" ref="AH4:AH6" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="AH4:AH6"/>
   <sortState ref="AH5:AH6">
     <sortCondition ref="AH4:AH6"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name=" سرمایه گذاری" dataDxfId="70"/>
+    <tableColumn id="1" name=" سرمایه گذاری" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="34" name="TravelAndTourExpensesTable" displayName="TravelAndTourExpensesTable" ref="AJ4:AJ6" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="34" name="TravelAndTourExpensesTable" displayName="TravelAndTourExpensesTable" ref="AJ4:AJ6" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <autoFilter ref="AJ4:AJ6"/>
   <sortState ref="AJ4">
     <sortCondition ref="AJ3:AJ4"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="سفر و گردش" dataDxfId="67"/>
+    <tableColumn id="1" name="سفر و گردش" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="HousingBillCostsTable" displayName="HousingBillCostsTable" ref="AL4:AL15" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="HousingBillCostsTable" displayName="HousingBillCostsTable" ref="AL4:AL15" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="AL4:AL15"/>
   <sortState ref="AL4:AL14">
     <sortCondition ref="AL3:AL14"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="صورتحاب‌های مسکن" dataDxfId="64"/>
+    <tableColumn id="1" name="صورتحاب‌های مسکن" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="SalaryTable" displayName="SalaryTable" ref="F5:F6" totalsRowShown="0" headerRowDxfId="144" dataDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="SalaryTable" displayName="SalaryTable" ref="F5:F6" totalsRowShown="0" headerRowDxfId="145" dataDxfId="144">
   <autoFilter ref="F5:F6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="دستمزد" dataDxfId="142"/>
+    <tableColumn id="1" name="دستمزد" dataDxfId="143"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="36" name="LeisureAndEntertainmentExpensesTable" displayName="LeisureAndEntertainmentExpensesTable" ref="AN4:AN8" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="36" name="LeisureAndEntertainmentExpensesTable" displayName="LeisureAndEntertainmentExpensesTable" ref="AN4:AN8" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
   <autoFilter ref="AN4:AN8"/>
   <sortState ref="AN4:AN7">
     <sortCondition ref="AN3:AN7"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="فراغت و سرگرمی" dataDxfId="61"/>
+    <tableColumn id="1" name="فراغت و سرگرمی" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="TaxCostsTable" displayName="TaxCostsTable" ref="AP4:AP8" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="TaxCostsTable" displayName="TaxCostsTable" ref="AP4:AP8" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="AP4:AP8"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="مالیات" dataDxfId="58"/>
+    <tableColumn id="1" name="مالیات" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="38" name="DegreeAndTuitionFeesTable" displayName="DegreeAndTuitionFeesTable" ref="AR4:AR6" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="38" name="DegreeAndTuitionFeesTable" displayName="DegreeAndTuitionFeesTable" ref="AR4:AR6" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="AR4:AR6"/>
   <sortState ref="AR4">
     <sortCondition ref="AR3:AR4"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name=" مدرک و تحصیل" dataDxfId="55"/>
+    <tableColumn id="1" name=" مدرک و تحصیل" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="39" name="ExerciseCostsTable" displayName="ExerciseCostsTable" ref="AT4:AT7" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="39" name="ExerciseCostsTable" displayName="ExerciseCostsTable" ref="AT4:AT7" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="AT4:AT7"/>
   <sortState ref="AT4:AT6">
     <sortCondition ref="AT3:AT6"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="ورزش" dataDxfId="52"/>
+    <tableColumn id="1" name="ورزش" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="40" name="GiftCostsTable" displayName="GiftCostsTable" ref="AV4:AV11" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="40" name="GiftCostsTable" displayName="GiftCostsTable" ref="AV4:AV11" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="AV4:AV11"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="هدیه و کادو" dataDxfId="49"/>
+    <tableColumn id="1" name="هدیه و کادو" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="LearningAndIndividualDevelopmentCostsTable" displayName="LearningAndIndividualDevelopmentCostsTable" ref="AX4:AX7" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="LearningAndIndividualDevelopmentCostsTable" displayName="LearningAndIndividualDevelopmentCostsTable" ref="AX4:AX7" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="AX4:AX7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="یادگیری و توسعه فردی" dataDxfId="46"/>
+    <tableColumn id="1" name="یادگیری و توسعه فردی" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ReceiversAndPayersTable" displayName="ReceiversAndPayersTable" ref="A3:A14" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ReceiversAndPayersTable" displayName="ReceiversAndPayersTable" ref="A3:A14" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" dataCellStyle="Normal">
   <autoFilter ref="A3:A14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="دریافت کننده - پرداخت کنندگان" dataDxfId="43" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="دریافت کننده - پرداخت کنندگان" dataDxfId="44" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Accounts_and_ReceiversAndPayers_AppendTabel" displayName="Accounts_and_ReceiversAndPayers_AppendTabel" ref="C3:E19" tableType="queryTable" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Accounts_and_ReceiversAndPayers_AppendTabel" displayName="Accounts_and_ReceiversAndPayers_AppendTabel" ref="C3:E19" tableType="queryTable" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="C3:E19"/>
   <tableColumns count="3">
-    <tableColumn id="4" uniqueName="4" name="Accounts" queryTableFieldId="1" dataDxfId="40"/>
-    <tableColumn id="5" uniqueName="5" name="ReceiversAndPayers" queryTableFieldId="2" dataDxfId="39"/>
-    <tableColumn id="6" uniqueName="6" name="Accounts and ReceiversAndPayers" queryTableFieldId="3" dataDxfId="38"/>
+    <tableColumn id="4" uniqueName="4" name="Accounts" queryTableFieldId="1" dataDxfId="41"/>
+    <tableColumn id="5" uniqueName="5" name="ReceiversAndPayers" queryTableFieldId="2" dataDxfId="40"/>
+    <tableColumn id="6" uniqueName="6" name="Accounts and ReceiversAndPayers" queryTableFieldId="3" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table38.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="PersonsTable" displayName="PersonsTable" ref="A5:I6" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="PersonsTable" displayName="PersonsTable" ref="A5:I6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A5:I6"/>
   <tableColumns count="9">
-    <tableColumn id="6" name="ID" dataDxfId="35"/>
-    <tableColumn id="1" name="افراد" dataDxfId="34"/>
-    <tableColumn id="2" name="کد ملی" dataDxfId="33"/>
-    <tableColumn id="3" name="شماره تماس" dataDxfId="32"/>
-    <tableColumn id="4" name="آدرس ایمیل" dataDxfId="31" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="سایت اینترنتی" dataDxfId="30"/>
-    <tableColumn id="7" name="آدرس محل کار" dataDxfId="29"/>
-    <tableColumn id="8" name="آدرس منزل" dataDxfId="28"/>
-    <tableColumn id="9" name="توضیحات" dataDxfId="27"/>
+    <tableColumn id="6" name="ID" dataDxfId="36"/>
+    <tableColumn id="1" name="افراد" dataDxfId="35"/>
+    <tableColumn id="2" name="کد ملی" dataDxfId="34"/>
+    <tableColumn id="3" name="شماره تماس" dataDxfId="33"/>
+    <tableColumn id="4" name="آدرس ایمیل" dataDxfId="32" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="سایت اینترنتی" dataDxfId="31"/>
+    <tableColumn id="7" name="آدرس محل کار" dataDxfId="30"/>
+    <tableColumn id="8" name="آدرس منزل" dataDxfId="29"/>
+    <tableColumn id="9" name="توضیحات" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FinancialAccountsTable" displayName="FinancialAccountsTable" ref="A12:L18" totalsRowCount="1" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FinancialAccountsTable" displayName="FinancialAccountsTable" ref="A12:L18" totalsRowCount="1" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A12:L17"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="ID" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="12"/>
-    <tableColumn id="2" name="نام حساب" dataDxfId="17" totalsRowDxfId="11"/>
-    <tableColumn id="3" name="نوع حساب" dataDxfId="16" totalsRowDxfId="10"/>
-    <tableColumn id="4" name="موجودی اولیه" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="9"/>
-    <tableColumn id="5" name="شماره حساب" totalsRowDxfId="8"/>
-    <tableColumn id="6" name="شماره کارت" totalsRowDxfId="7"/>
-    <tableColumn id="7" name="تاریخ انقضاء کارت" totalsRowDxfId="6"/>
-    <tableColumn id="8" name="CVV2" totalsRowDxfId="5"/>
-    <tableColumn id="9" name="جمع پرداختی" totalsRowFunction="sum" totalsRowDxfId="2">
+    <tableColumn id="1" name="ID" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="نام حساب" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="نوع حساب" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="موجودی اولیه" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="شماره حساب" totalsRowDxfId="17"/>
+    <tableColumn id="6" name="شماره کارت" totalsRowDxfId="16"/>
+    <tableColumn id="7" name="تاریخ انقضاء کارت" totalsRowDxfId="15"/>
+    <tableColumn id="8" name="CVV2" totalsRowDxfId="14"/>
+    <tableColumn id="9" name="جمع پرداختی" totalsRowFunction="sum" totalsRowDxfId="13">
       <calculatedColumnFormula>SUMIF(Tarakonesh[پرداخت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="جمع دریافتی" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="1">
+    <tableColumn id="11" name="جمع دریافتی" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11">
       <calculatedColumnFormula>SUMIF(Tarakonesh[دریافت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="مانده" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="0">
+    <tableColumn id="12" name="مانده" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>(FinancialAccountsTable[[#This Row],[جمع دریافتی]]+FinancialAccountsTable[[#This Row],[موجودی اولیه]])-FinancialAccountsTable[[#This Row],[جمع پرداختی]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="وضعیت فعلی" dataDxfId="3" totalsRowDxfId="4">
+    <tableColumn id="13" name="وضعیت فعلی" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>IF(FinancialAccountsTable[[#This Row],[مانده]]=0,"",IF(FinancialAccountsTable[[#This Row],[مانده]]&gt;0,"بدهکار","بستانکار"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4466,30 +4476,30 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="ProfitOfAcquisitionTable" displayName="ProfitOfAcquisitionTable" ref="H5:H6" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="ProfitOfAcquisitionTable" displayName="ProfitOfAcquisitionTable" ref="H5:H6" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141">
   <autoFilter ref="H5:H6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="منفعت کسب" dataDxfId="139"/>
+    <tableColumn id="1" name="منفعت کسب" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table40.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TypeOfExpenditureTable" displayName="TypeOfExpenditureTable" ref="A3:A6" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TypeOfExpenditureTable" displayName="TypeOfExpenditureTable" ref="A3:A6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A3:A6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="نوع خرج" dataDxfId="24"/>
+    <tableColumn id="1" name="نوع خرج" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table41.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TypeOfTransactionTable" displayName="TypeOfTransactionTable" ref="B3:B6" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TypeOfTransactionTable" displayName="TypeOfTransactionTable" ref="B3:B6" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="B3:B6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="نوع تراکنش" dataDxfId="21"/>
+    <tableColumn id="1" name="نوع تراکنش" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4506,53 +4516,53 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="ProfitableInvestmentTable" displayName="ProfitableInvestmentTable" ref="J5:J6" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="ProfitableInvestmentTable" displayName="ProfitableInvestmentTable" ref="J5:J6" totalsRowShown="0" headerRowDxfId="139" dataDxfId="138">
   <autoFilter ref="J5:J6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="سود سرمایه‌گذاری" dataDxfId="136"/>
+    <tableColumn id="1" name="سود سرمایه‌گذاری" dataDxfId="137"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="IncentivesPrizesAndFeastsTable" displayName="IncentivesPrizesAndFeastsTable" ref="L5:L8" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="IncentivesPrizesAndFeastsTable" displayName="IncentivesPrizesAndFeastsTable" ref="L5:L8" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135">
   <autoFilter ref="L5:L8"/>
   <sortState ref="L6:L8">
     <sortCondition ref="L5:L8"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="تشویقی‌ها، جوایز و عیدی‌ها" dataDxfId="133"/>
+    <tableColumn id="1" name="تشویقی‌ها، جوایز و عیدی‌ها" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="GetAMortgageAndRentTable" displayName="GetAMortgageAndRentTable" ref="N5:N6" totalsRowShown="0" headerRowDxfId="132" dataDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="GetAMortgageAndRentTable" displayName="GetAMortgageAndRentTable" ref="N5:N6" totalsRowShown="0" headerRowDxfId="133" dataDxfId="132">
   <autoFilter ref="N5:N6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="دریافت رهن و اجاره" dataDxfId="130"/>
+    <tableColumn id="1" name="دریافت رهن و اجاره" dataDxfId="131"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="GetALoanTable" displayName="GetALoanTable" ref="P5:P6" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="GetALoanTable" displayName="GetALoanTable" ref="P5:P6" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129">
   <autoFilter ref="P5:P6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="دریافت وام" dataDxfId="127"/>
+    <tableColumn id="1" name="دریافت وام" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="MiscellaneousIncomeTable" displayName="MiscellaneousIncomeTable" ref="R5:R6" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="MiscellaneousIncomeTable" displayName="MiscellaneousIncomeTable" ref="R5:R6" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
   <autoFilter ref="R5:R6"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="درآمد متفرقه" dataDxfId="124"/>
+    <tableColumn id="1" name="درآمد متفرقه" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4821,10 +4831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AC16"/>
+  <dimension ref="A4:AC22"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O3:AC12"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5069,9 +5079,15 @@
         <v>99</v>
       </c>
     </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>351</v>
+      </c>
+    </row>
     <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>8</v>
+      <c r="A16" s="11" t="e">
+        <f>S24a</f>
+        <v>#NAME?</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>120</v>
@@ -5100,9 +5116,44 @@
       <c r="J16" s="17" t="s">
         <v>99</v>
       </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="U16" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="17" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <f>IF(Q16:Q22="",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
+  <dataValidations disablePrompts="1" count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V8">
       <formula1>INDIRECT($F$10)</formula1>
     </dataValidation>
@@ -5409,10 +5460,10 @@
     </row>
     <row r="2" spans="1:23" s="43" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="125" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="119"/>
+      <c r="B3" s="125"/>
       <c r="D3" s="43"/>
       <c r="F3" s="43"/>
       <c r="H3" s="43"/>
@@ -5837,10 +5888,10 @@
       <c r="AC3" s="90"/>
     </row>
     <row r="4" spans="1:55" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="120" t="s">
+      <c r="A4" s="126" t="s">
         <v>176</v>
       </c>
-      <c r="B4" s="120"/>
+      <c r="B4" s="126"/>
       <c r="D4" s="45" t="s">
         <v>194</v>
       </c>
@@ -7885,7 +7936,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8061,15 +8112,15 @@
       <c r="H13" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="122">
+      <c r="I13" s="119">
         <f>SUMIF(Tarakonesh[پرداخت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>20000</v>
       </c>
-      <c r="J13" s="122">
+      <c r="J13" s="119">
         <f>SUMIF(Tarakonesh[دریافت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>500000</v>
       </c>
-      <c r="K13" s="122">
+      <c r="K13" s="119">
         <f>(FinancialAccountsTable[[#This Row],[جمع دریافتی]]+FinancialAccountsTable[[#This Row],[موجودی اولیه]])-FinancialAccountsTable[[#This Row],[جمع پرداختی]]</f>
         <v>2480000</v>
       </c>
@@ -8101,15 +8152,15 @@
       <c r="H14" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="122">
+      <c r="I14" s="119">
         <f>SUMIF(Tarakonesh[پرداخت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>80000</v>
       </c>
-      <c r="J14" s="122">
+      <c r="J14" s="119">
         <f>SUMIF(Tarakonesh[دریافت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>1020000</v>
       </c>
-      <c r="K14" s="122">
+      <c r="K14" s="119">
         <f>(FinancialAccountsTable[[#This Row],[جمع دریافتی]]+FinancialAccountsTable[[#This Row],[موجودی اولیه]])-FinancialAccountsTable[[#This Row],[جمع پرداختی]]</f>
         <v>940000</v>
       </c>
@@ -8139,15 +8190,15 @@
       <c r="H15" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="I15" s="122">
+      <c r="I15" s="119">
         <f>SUMIF(Tarakonesh[پرداخت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>3000</v>
       </c>
-      <c r="J15" s="122">
+      <c r="J15" s="119">
         <f>SUMIF(Tarakonesh[دریافت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>520000</v>
       </c>
-      <c r="K15" s="122">
+      <c r="K15" s="119">
         <f>(FinancialAccountsTable[[#This Row],[جمع دریافتی]]+FinancialAccountsTable[[#This Row],[موجودی اولیه]])-FinancialAccountsTable[[#This Row],[جمع پرداختی]]</f>
         <v>517000</v>
       </c>
@@ -8177,15 +8228,15 @@
       <c r="H16" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="I16" s="122">
+      <c r="I16" s="119">
         <f>SUMIF(Tarakonesh[پرداخت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>500000</v>
       </c>
-      <c r="J16" s="122">
+      <c r="J16" s="119">
         <f>SUMIF(Tarakonesh[دریافت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>0</v>
       </c>
-      <c r="K16" s="122">
+      <c r="K16" s="119">
         <f>(FinancialAccountsTable[[#This Row],[جمع دریافتی]]+FinancialAccountsTable[[#This Row],[موجودی اولیه]])-FinancialAccountsTable[[#This Row],[جمع پرداختی]]</f>
         <v>-500000</v>
       </c>
@@ -8213,15 +8264,15 @@
       <c r="H17" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="I17" s="122">
+      <c r="I17" s="119">
         <f>SUMIF(Tarakonesh[پرداخت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>0</v>
       </c>
-      <c r="J17" s="122">
+      <c r="J17" s="119">
         <f>SUMIF(Tarakonesh[دریافت کننده],FinancialAccountsTable[[#This Row],[نام حساب]],Tarakonesh[مبلغ (ریال)])</f>
         <v>0</v>
       </c>
-      <c r="K17" s="122">
+      <c r="K17" s="119">
         <f>(FinancialAccountsTable[[#This Row],[جمع دریافتی]]+FinancialAccountsTable[[#This Row],[موجودی اولیه]])-FinancialAccountsTable[[#This Row],[جمع پرداختی]]</f>
         <v>0</v>
       </c>
@@ -8244,15 +8295,15 @@
       <c r="F18" s="69"/>
       <c r="G18" s="70"/>
       <c r="H18" s="70"/>
-      <c r="I18" s="123">
+      <c r="I18" s="120">
         <f>SUBTOTAL(109,FinancialAccountsTable[جمع پرداختی])</f>
         <v>603000</v>
       </c>
-      <c r="J18" s="123">
+      <c r="J18" s="120">
         <f>SUBTOTAL(109,FinancialAccountsTable[جمع دریافتی])</f>
         <v>2040000</v>
       </c>
-      <c r="K18" s="123">
+      <c r="K18" s="120">
         <f>SUBTOTAL(109,FinancialAccountsTable[مانده])</f>
         <v>3437000</v>
       </c>
@@ -8551,7 +8602,7 @@
   <dimension ref="A1:S507"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8604,7 +8655,9 @@
       <c r="J1" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="6"/>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="L1" s="6"/>
       <c r="M1" s="30"/>
       <c r="N1" s="6"/>
@@ -8638,29 +8691,29 @@
       <c r="B3" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="126">
+      <c r="C3" s="123">
         <f>SUMIF(Tarakonesh[تراکنش],"دریافت_درآمد",Tarakonesh[مبلغ (ریال)])</f>
         <v>1520000</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="125">
+      <c r="E3" s="122">
         <f>SUMIF(Tarakonesh[تراکنش],"پرداخت_هزینه",Tarakonesh[مبلغ (ریال)])</f>
-        <v>83000</v>
+        <v>93000</v>
       </c>
       <c r="F3" s="39" t="s">
         <v>349</v>
       </c>
-      <c r="G3" s="124">
+      <c r="G3" s="121">
         <f>SUMIF(Tarakonesh[تراکنش],"انتقال",Tarakonesh[مبلغ (ریال)])</f>
         <v>520000</v>
       </c>
       <c r="H3" s="86"/>
-      <c r="I3" s="118" t="s">
+      <c r="I3" s="124" t="s">
         <v>154</v>
       </c>
-      <c r="J3" s="118"/>
+      <c r="J3" s="124"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="31"/>
@@ -8697,7 +8750,7 @@
       </c>
       <c r="C5" s="85">
         <f ca="1">TODAY()</f>
-        <v>44425</v>
+        <v>44426</v>
       </c>
       <c r="D5" s="79"/>
       <c r="E5" s="80"/>
@@ -8823,7 +8876,10 @@
       <c r="K8" s="29" t="s">
         <v>342</v>
       </c>
-      <c r="L8" s="29"/>
+      <c r="L8" s="29">
+        <f>IF( Tarakonesh[تراکنش]="", "",IF( Tarakonesh[تراکنش]="انتقال", "",(FinancialAccountsTable[[#Totals],[موجودی اولیه]] + IF(Tarakonesh[تراکنش]="دریافت_درآمد",Tarakonesh[[#This Row],[مبلغ (ریال)]],0))-IF(Tarakonesh[تراکنش]="پرداخت_هزینه",Tarakonesh[[#This Row],[مبلغ (ریال)]],0)))</f>
+        <v>1920000</v>
+      </c>
       <c r="M8" s="33" t="s">
         <v>118</v>
       </c>
@@ -8860,7 +8916,10 @@
       <c r="K9" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="L9" s="29"/>
+      <c r="L9" s="29">
+        <f>IF( Tarakonesh[تراکنش]="", "",IF( Tarakonesh[تراکنش]="انتقال", "",IF(Tarakonesh[تراکنش]="دریافت_درآمد",Tarakonesh[[#This Row],[مبلغ (ریال)]]+IF(Tarakonesh[تراکنش]="انتقال",0,L8),Tarakonesh[[#This Row],[مبلغ (ریال)]]-IF(Tarakonesh[تراکنش]="انتقال",0,L8))))</f>
+        <v>2920000</v>
+      </c>
       <c r="M9" s="33"/>
       <c r="N9" s="33"/>
     </row>
@@ -8894,7 +8953,7 @@
       <c r="L10" s="29"/>
       <c r="M10" s="33"/>
       <c r="N10" s="33"/>
-      <c r="R10" s="121"/>
+      <c r="R10" s="118"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
@@ -8927,7 +8986,7 @@
       <c r="L11" s="29"/>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
-      <c r="R11" s="121"/>
+      <c r="R11" s="118"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
@@ -9014,11 +9073,15 @@
       <c r="B15" s="29"/>
       <c r="C15" s="77"/>
       <c r="D15" s="33"/>
-      <c r="E15" s="41"/>
+      <c r="E15" s="41" t="s">
+        <v>291</v>
+      </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
-      <c r="I15" s="27"/>
+      <c r="I15" s="27">
+        <v>10000</v>
+      </c>
       <c r="J15" s="29"/>
       <c r="K15" s="29"/>
       <c r="L15" s="29"/>
@@ -17941,6 +18004,7 @@
     <hyperlink ref="I3:J3" location="'دریافت کنندگان - پرداخت کنندگان'!A1" display="دریافت کنندگان - پرداخت کنندگان"/>
     <hyperlink ref="I5" location="'گروه‌‌های (بابت‌ها) هزینه'!A1" display="گروه‌های هزینه"/>
     <hyperlink ref="J5" location="'گروه‌‌های درآمدی'!A1" display="گروه‌های درآمد"/>
+    <hyperlink ref="K1" location="'تنظیمات حساب'!A1" display="تنظیمات حساب"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>